<commit_message>
fixed the clickable area in the main radar chart
</commit_message>
<xml_diff>
--- a/radar_chart_coords.xlsx
+++ b/radar_chart_coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseulloa/Developer/maqueta_ines_genero/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3173381-9221-9843-8847-AFE70CA9A83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB912AD-FDCF-F44C-A484-AFC1F01C2160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1600" windowWidth="27640" windowHeight="16940" xr2:uid="{959BF0BF-7833-C840-AD88-51CDC2D134D8}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{959BF0BF-7833-C840-AD88-51CDC2D134D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Centre</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>shift</t>
+  </si>
+  <si>
+    <t>Image Size:</t>
   </si>
 </sst>
 </file>
@@ -227,25 +230,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>157.73817382593009</c:v>
+                  <c:v>473.35808591116103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>244.50817844365926</c:v>
+                  <c:v>1514.5981413239112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>297.76261689193046</c:v>
+                  <c:v>2153.6514027031653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>277.39981082662274</c:v>
+                  <c:v>1909.2977299194731</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>198.75336854045847</c:v>
+                  <c:v>965.54042248550172</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121.04566516997643</c:v>
+                  <c:v>33.047982039717226</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>102.79218630142253</c:v>
+                  <c:v>-185.99376438292961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -257,25 +260,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>89.369221296334999</c:v>
+                  <c:v>-194.06934444398007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.451007534269905</c:v>
+                  <c:v>-181.08790958876102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>158.96501156545045</c:v>
+                  <c:v>641.08013878540544</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>243.31879092341396</c:v>
+                  <c:v>1653.3254910809674</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>279.99222924809749</c:v>
+                  <c:v>2093.4067509771698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>241.3694794792047</c:v>
+                  <c:v>1629.9337537504566</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>156.53425995322851</c:v>
+                  <c:v>611.91111943874239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1388,23 +1391,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D4F019-0D23-9341-A4AF-84B12785EB4C}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>200</v>
+        <f>J1/2</f>
+        <v>980.5</v>
       </c>
       <c r="C1">
-        <v>180</v>
+        <f>J2/2</f>
+        <v>893.5</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1412,13 +1417,19 @@
       <c r="F1">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>1200</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -1427,8 +1438,11 @@
         <f>360/F1</f>
         <v>51.428571428571431</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>8</v>
       </c>
@@ -1436,7 +1450,7 @@
         <v>-115</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1450,7 +1464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1460,26 +1474,26 @@
       </c>
       <c r="C5" s="1">
         <f>$B$1 + $B$2*COS(RADIANS(B5))</f>
-        <v>157.73817382593009</v>
+        <v>473.35808591116103</v>
       </c>
       <c r="D5" s="1">
         <f>$C$1 + $B$2*SIN(RADIANS(B5))</f>
-        <v>89.369221296334999</v>
+        <v>-194.06934444398007</v>
       </c>
       <c r="F5" t="str">
         <f>TEXT(C5,0)&amp;","&amp;TEXT(D5,0)</f>
-        <v>158,89</v>
+        <v>473,-194</v>
       </c>
       <c r="G5" t="str">
         <f>F6</f>
-        <v>245,90</v>
+        <v>1515,-181</v>
       </c>
       <c r="H5" t="str">
         <f>$B$1&amp;","&amp;$C$1</f>
-        <v>200,180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>980.5,893.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1489,26 +1503,26 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:C11" si="1">$B$1 + $B$2*COS(RADIANS(B6))</f>
-        <v>244.50817844365926</v>
+        <v>1514.5981413239112</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6:D11" si="2">$C$1 + $B$2*SIN(RADIANS(B6))</f>
-        <v>90.451007534269905</v>
+        <v>-181.08790958876102</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ref="F6:F11" si="3">TEXT(C6,0)&amp;","&amp;TEXT(D6,0)</f>
-        <v>245,90</v>
+        <v>1515,-181</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" ref="G6:G11" si="4">F7</f>
-        <v>298,159</v>
+        <f t="shared" ref="G6:G10" si="4">F7</f>
+        <v>2154,641</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ref="H6:H11" si="5">$B$1&amp;","&amp;$C$1</f>
-        <v>200,180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>980.5,893.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1518,26 +1532,26 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>297.76261689193046</v>
+        <v>2153.6514027031653</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>158.96501156545045</v>
+        <v>641.08013878540544</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="3"/>
-        <v>298,159</v>
+        <v>2154,641</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="4"/>
-        <v>277,243</v>
+        <v>1909,1653</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="5"/>
-        <v>200,180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>980.5,893.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1547,26 +1561,26 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>277.39981082662274</v>
+        <v>1909.2977299194731</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>243.31879092341396</v>
+        <v>1653.3254910809674</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="3"/>
-        <v>277,243</v>
+        <v>1909,1653</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="4"/>
-        <v>199,280</v>
+        <v>966,2093</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="5"/>
-        <v>200,180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>980.5,893.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1576,26 +1590,26 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>198.75336854045847</v>
+        <v>965.54042248550172</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>279.99222924809749</v>
+        <v>2093.4067509771698</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="3"/>
-        <v>199,280</v>
+        <v>966,2093</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="4"/>
-        <v>121,241</v>
+        <v>33,1630</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="5"/>
-        <v>200,180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>980.5,893.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1605,26 +1619,26 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>121.04566516997643</v>
+        <v>33.047982039717226</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>241.3694794792047</v>
+        <v>1629.9337537504566</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="3"/>
-        <v>121,241</v>
+        <v>33,1630</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="4"/>
-        <v>103,157</v>
+        <v>-186,612</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="5"/>
-        <v>200,180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>980.5,893.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1634,59 +1648,59 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>102.79218630142253</v>
+        <v>-185.99376438292961</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>156.53425995322851</v>
+        <v>611.91111943874239</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="3"/>
-        <v>103,157</v>
+        <v>-186,612</v>
       </c>
       <c r="G11" t="str">
         <f>F5</f>
-        <v>158,89</v>
+        <v>473,-194</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="5"/>
-        <v>200,180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>980.5,893.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="str">
         <f>F5&amp;", "&amp;G5&amp;", "&amp;H5</f>
-        <v>158,89, 245,90, 200,180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>473,-194, 1515,-181, 980.5,893.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" ref="F14:F20" si="6">F6&amp;", "&amp;G6&amp;", "&amp;H6</f>
-        <v>245,90, 298,159, 200,180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F14:F18" si="6">F6&amp;", "&amp;G6&amp;", "&amp;H6</f>
+        <v>1515,-181, 2154,641, 980.5,893.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="6"/>
-        <v>298,159, 277,243, 200,180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2154,641, 1909,1653, 980.5,893.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E16">
         <v>4</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="6"/>
-        <v>277,243, 199,280, 200,180</v>
+        <v>1909,1653, 966,2093, 980.5,893.5</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.2">
@@ -1695,7 +1709,7 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="6"/>
-        <v>199,280, 121,241, 200,180</v>
+        <v>966,2093, 33,1630, 980.5,893.5</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.2">
@@ -1704,7 +1718,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="6"/>
-        <v>121,241, 103,157, 200,180</v>
+        <v>33,1630, -186,612, 980.5,893.5</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
@@ -1713,49 +1727,49 @@
       </c>
       <c r="F19" t="str">
         <f>F11&amp;", "&amp;G11&amp;", "&amp;H11</f>
-        <v>103,157, 158,89, 200,180</v>
+        <v>-186,612, 473,-194, 980.5,893.5</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D21" t="str">
         <f>"&lt;area shape=""poly"" coords="""&amp;F13&amp;""" href=""#"" alt=""Heptagon Section "&amp;E13&amp;""" data-popup=""popup"&amp;E13&amp;"""/&gt;"</f>
-        <v>&lt;area shape="poly" coords="158,89, 245,90, 200,180" href="#" alt="Heptagon Section 1" data-popup="popup1"/&gt;</v>
+        <v>&lt;area shape="poly" coords="473,-194, 1515,-181, 980.5,893.5" href="#" alt="Heptagon Section 1" data-popup="popup1"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D22" t="str">
         <f t="shared" ref="D22:D27" si="7">"&lt;area shape=""poly"" coords="""&amp;F14&amp;""" href=""#"" alt=""Heptagon Section "&amp;E14&amp;""" data-popup=""popup"&amp;E14&amp;"""/&gt;"</f>
-        <v>&lt;area shape="poly" coords="245,90, 298,159, 200,180" href="#" alt="Heptagon Section 2" data-popup="popup2"/&gt;</v>
+        <v>&lt;area shape="poly" coords="1515,-181, 2154,641, 980.5,893.5" href="#" alt="Heptagon Section 2" data-popup="popup2"/&gt;</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D23" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="298,159, 277,243, 200,180" href="#" alt="Heptagon Section 3" data-popup="popup3"/&gt;</v>
+        <v>&lt;area shape="poly" coords="2154,641, 1909,1653, 980.5,893.5" href="#" alt="Heptagon Section 3" data-popup="popup3"/&gt;</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D24" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="277,243, 199,280, 200,180" href="#" alt="Heptagon Section 4" data-popup="popup4"/&gt;</v>
+        <v>&lt;area shape="poly" coords="1909,1653, 966,2093, 980.5,893.5" href="#" alt="Heptagon Section 4" data-popup="popup4"/&gt;</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D25" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="199,280, 121,241, 200,180" href="#" alt="Heptagon Section 5" data-popup="popup5"/&gt;</v>
+        <v>&lt;area shape="poly" coords="966,2093, 33,1630, 980.5,893.5" href="#" alt="Heptagon Section 5" data-popup="popup5"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D26" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="121,241, 103,157, 200,180" href="#" alt="Heptagon Section 6" data-popup="popup6"/&gt;</v>
+        <v>&lt;area shape="poly" coords="33,1630, -186,612, 980.5,893.5" href="#" alt="Heptagon Section 6" data-popup="popup6"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D27" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="103,157, 158,89, 200,180" href="#" alt="Heptagon Section 7" data-popup="popup7"/&gt;</v>
+        <v>&lt;area shape="poly" coords="-186,612, 473,-194, 980.5,893.5" href="#" alt="Heptagon Section 7" data-popup="popup7"/&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final update to submit for review
</commit_message>
<xml_diff>
--- a/radar_chart_coords.xlsx
+++ b/radar_chart_coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseulloa/Developer/maqueta_ines_genero/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB912AD-FDCF-F44C-A484-AFC1F01C2160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF7863-BD53-FF4C-BDD1-00DE8CC5407F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{959BF0BF-7833-C840-AD88-51CDC2D134D8}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="33420" windowHeight="18060" xr2:uid="{959BF0BF-7833-C840-AD88-51CDC2D134D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Centre</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Image Size:</t>
+  </si>
+  <si>
+    <t>7260 × 6237</t>
   </si>
 </sst>
 </file>
@@ -230,25 +233,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>473.35808591116103</c:v>
+                  <c:v>1178.814081903945</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1514.5981413239112</c:v>
+                  <c:v>6211.4743497322379</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2153.6514027031653</c:v>
+                  <c:v>9300.2317797319665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1909.2977299194731</c:v>
+                  <c:v>8119.1890279441204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>965.54042248550172</c:v>
+                  <c:v>3557.6953753465914</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.047982039717226</c:v>
+                  <c:v>-949.35142014136636</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-185.99376438292961</c:v>
+                  <c:v>-2008.0531945174935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -260,25 +263,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>-194.06934444398007</c:v>
+                  <c:v>-2138.0851648125699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-181.08790958876102</c:v>
+                  <c:v>-2075.3415630123454</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>641.08013878540544</c:v>
+                  <c:v>1898.4706707961263</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1653.3254910809674</c:v>
+                  <c:v>6790.98987355801</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2093.4067509771698</c:v>
+                  <c:v>8918.049296389654</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1629.9337537504566</c:v>
+                  <c:v>6677.9298097938736</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>611.91111943874239</c:v>
+                  <c:v>1757.4870772872546</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,25 +1394,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D4F019-0D23-9341-A4AF-84B12785EB4C}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <f>J1/2</f>
-        <v>980.5</v>
+        <v>3630</v>
       </c>
       <c r="C1">
         <f>J2/2</f>
-        <v>893.5</v>
+        <v>3118.5</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -1421,15 +1424,19 @@
         <v>9</v>
       </c>
       <c r="J1">
-        <v>1961</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>7260</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1200</v>
+        <f>MROUND(0.8*J4, 100)</f>
+        <v>5800</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -1439,10 +1446,10 @@
         <v>51.428571428571431</v>
       </c>
       <c r="J2">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>8</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>-115</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1463,8 +1470,12 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <f>MAX(J1:J2)</f>
+        <v>7260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1474,26 +1485,26 @@
       </c>
       <c r="C5" s="1">
         <f>$B$1 + $B$2*COS(RADIANS(B5))</f>
-        <v>473.35808591116103</v>
+        <v>1178.814081903945</v>
       </c>
       <c r="D5" s="1">
         <f>$C$1 + $B$2*SIN(RADIANS(B5))</f>
-        <v>-194.06934444398007</v>
+        <v>-2138.0851648125699</v>
       </c>
       <c r="F5" t="str">
         <f>TEXT(C5,0)&amp;","&amp;TEXT(D5,0)</f>
-        <v>473,-194</v>
+        <v>1179,-2138</v>
       </c>
       <c r="G5" t="str">
         <f>F6</f>
-        <v>1515,-181</v>
+        <v>6211,-2075</v>
       </c>
       <c r="H5" t="str">
         <f>$B$1&amp;","&amp;$C$1</f>
-        <v>980.5,893.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3630,3118.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1503,26 +1514,26 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:C11" si="1">$B$1 + $B$2*COS(RADIANS(B6))</f>
-        <v>1514.5981413239112</v>
+        <v>6211.4743497322379</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6:D11" si="2">$C$1 + $B$2*SIN(RADIANS(B6))</f>
-        <v>-181.08790958876102</v>
+        <v>-2075.3415630123454</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ref="F6:F11" si="3">TEXT(C6,0)&amp;","&amp;TEXT(D6,0)</f>
-        <v>1515,-181</v>
+        <v>6211,-2075</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ref="G6:G10" si="4">F7</f>
-        <v>2154,641</v>
+        <v>9300,1898</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ref="H6:H11" si="5">$B$1&amp;","&amp;$C$1</f>
-        <v>980.5,893.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3630,3118.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1532,26 +1543,26 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>2153.6514027031653</v>
+        <v>9300.2317797319665</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>641.08013878540544</v>
+        <v>1898.4706707961263</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="3"/>
-        <v>2154,641</v>
+        <v>9300,1898</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="4"/>
-        <v>1909,1653</v>
+        <v>8119,6791</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="5"/>
-        <v>980.5,893.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3630,3118.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1561,26 +1572,26 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>1909.2977299194731</v>
+        <v>8119.1890279441204</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>1653.3254910809674</v>
+        <v>6790.98987355801</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="3"/>
-        <v>1909,1653</v>
+        <v>8119,6791</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="4"/>
-        <v>966,2093</v>
+        <v>3558,8918</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="5"/>
-        <v>980.5,893.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3630,3118.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1590,26 +1601,26 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>965.54042248550172</v>
+        <v>3557.6953753465914</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>2093.4067509771698</v>
+        <v>8918.049296389654</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="3"/>
-        <v>966,2093</v>
+        <v>3558,8918</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="4"/>
-        <v>33,1630</v>
+        <v>-949,6678</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="5"/>
-        <v>980.5,893.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3630,3118.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1619,26 +1630,26 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>33.047982039717226</v>
+        <v>-949.35142014136636</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>1629.9337537504566</v>
+        <v>6677.9298097938736</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="3"/>
-        <v>33,1630</v>
+        <v>-949,6678</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="4"/>
-        <v>-186,612</v>
+        <v>-2008,1757</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="5"/>
-        <v>980.5,893.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3630,3118.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1648,59 +1659,59 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>-185.99376438292961</v>
+        <v>-2008.0531945174935</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>611.91111943874239</v>
+        <v>1757.4870772872546</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="3"/>
-        <v>-186,612</v>
+        <v>-2008,1757</v>
       </c>
       <c r="G11" t="str">
         <f>F5</f>
-        <v>473,-194</v>
+        <v>1179,-2138</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="5"/>
-        <v>980.5,893.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3630,3118.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="str">
         <f>F5&amp;", "&amp;G5&amp;", "&amp;H5</f>
-        <v>473,-194, 1515,-181, 980.5,893.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1179,-2138, 6211,-2075, 3630,3118.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ref="F14:F18" si="6">F6&amp;", "&amp;G6&amp;", "&amp;H6</f>
-        <v>1515,-181, 2154,641, 980.5,893.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6211,-2075, 9300,1898, 3630,3118.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="6"/>
-        <v>2154,641, 1909,1653, 980.5,893.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9300,1898, 8119,6791, 3630,3118.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E16">
         <v>4</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="6"/>
-        <v>1909,1653, 966,2093, 980.5,893.5</v>
+        <v>8119,6791, 3558,8918, 3630,3118.5</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.2">
@@ -1709,7 +1720,7 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="6"/>
-        <v>966,2093, 33,1630, 980.5,893.5</v>
+        <v>3558,8918, -949,6678, 3630,3118.5</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.2">
@@ -1718,7 +1729,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="6"/>
-        <v>33,1630, -186,612, 980.5,893.5</v>
+        <v>-949,6678, -2008,1757, 3630,3118.5</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
@@ -1727,49 +1738,49 @@
       </c>
       <c r="F19" t="str">
         <f>F11&amp;", "&amp;G11&amp;", "&amp;H11</f>
-        <v>-186,612, 473,-194, 980.5,893.5</v>
+        <v>-2008,1757, 1179,-2138, 3630,3118.5</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D21" t="str">
         <f>"&lt;area shape=""poly"" coords="""&amp;F13&amp;""" href=""#"" alt=""Heptagon Section "&amp;E13&amp;""" data-popup=""popup"&amp;E13&amp;"""/&gt;"</f>
-        <v>&lt;area shape="poly" coords="473,-194, 1515,-181, 980.5,893.5" href="#" alt="Heptagon Section 1" data-popup="popup1"/&gt;</v>
+        <v>&lt;area shape="poly" coords="1179,-2138, 6211,-2075, 3630,3118.5" href="#" alt="Heptagon Section 1" data-popup="popup1"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D22" t="str">
         <f t="shared" ref="D22:D27" si="7">"&lt;area shape=""poly"" coords="""&amp;F14&amp;""" href=""#"" alt=""Heptagon Section "&amp;E14&amp;""" data-popup=""popup"&amp;E14&amp;"""/&gt;"</f>
-        <v>&lt;area shape="poly" coords="1515,-181, 2154,641, 980.5,893.5" href="#" alt="Heptagon Section 2" data-popup="popup2"/&gt;</v>
+        <v>&lt;area shape="poly" coords="6211,-2075, 9300,1898, 3630,3118.5" href="#" alt="Heptagon Section 2" data-popup="popup2"/&gt;</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D23" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="2154,641, 1909,1653, 980.5,893.5" href="#" alt="Heptagon Section 3" data-popup="popup3"/&gt;</v>
+        <v>&lt;area shape="poly" coords="9300,1898, 8119,6791, 3630,3118.5" href="#" alt="Heptagon Section 3" data-popup="popup3"/&gt;</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D24" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="1909,1653, 966,2093, 980.5,893.5" href="#" alt="Heptagon Section 4" data-popup="popup4"/&gt;</v>
+        <v>&lt;area shape="poly" coords="8119,6791, 3558,8918, 3630,3118.5" href="#" alt="Heptagon Section 4" data-popup="popup4"/&gt;</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D25" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="966,2093, 33,1630, 980.5,893.5" href="#" alt="Heptagon Section 5" data-popup="popup5"/&gt;</v>
+        <v>&lt;area shape="poly" coords="3558,8918, -949,6678, 3630,3118.5" href="#" alt="Heptagon Section 5" data-popup="popup5"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D26" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="33,1630, -186,612, 980.5,893.5" href="#" alt="Heptagon Section 6" data-popup="popup6"/&gt;</v>
+        <v>&lt;area shape="poly" coords="-949,6678, -2008,1757, 3630,3118.5" href="#" alt="Heptagon Section 6" data-popup="popup6"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D27" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;area shape="poly" coords="-186,612, 473,-194, 980.5,893.5" href="#" alt="Heptagon Section 7" data-popup="popup7"/&gt;</v>
+        <v>&lt;area shape="poly" coords="-2008,1757, 1179,-2138, 3630,3118.5" href="#" alt="Heptagon Section 7" data-popup="popup7"/&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>